<commit_message>
added pixel size equation
</commit_message>
<xml_diff>
--- a/results/marker_sizing/24-03-18_marker-sizing-test/24-03-18_marker-size-test-data.xlsx
+++ b/results/marker_sizing/24-03-18_marker-sizing-test/24-03-18_marker-size-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\downloads_current\24-03-18_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\documents\uvm\5_masters\hive\github_directory\results\marker_sizing\24-03-18_marker-sizing-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{288E0A4F-959B-4E49-BC7C-817B226DB64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52251818-BFC5-4F25-A082-CBEF155495D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{8CE0953D-CCFE-4D6F-99ED-C5F9A62F855B}"/>
+    <workbookView xWindow="13275" yWindow="20070" windowWidth="21600" windowHeight="11385" xr2:uid="{8CE0953D-CCFE-4D6F-99ED-C5F9A62F855B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>angle at max [deg]</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>marker size [mm]</t>
+  </si>
+  <si>
+    <t>expected pixel size</t>
+  </si>
+  <si>
+    <t>camera specs</t>
+  </si>
+  <si>
+    <t>image width [px]</t>
+  </si>
+  <si>
+    <t>FOV [rad]</t>
+  </si>
+  <si>
+    <t>actual pixel size (counted from image)</t>
   </si>
 </sst>
 </file>
@@ -1920,16 +1935,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1956,16 +1971,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2310,15 +2325,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E525651-0775-4550-ACDA-40153B2C3039}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2331,8 +2346,14 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30</v>
       </c>
@@ -2344,11 +2365,18 @@
         <v>3.3856810650317593E-2</v>
       </c>
       <c r="D2">
-        <f>C2*180/PI()</f>
+        <f>DEGREES(C2)</f>
         <v>1.9398523580367741</v>
       </c>
+      <c r="E2">
+        <f>A2*$A$10/(2*B2*TAN($A$11/2))</f>
+        <v>11.4179336373558</v>
+      </c>
+      <c r="F2">
+        <v>11.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>38</v>
       </c>
@@ -2360,11 +2388,18 @@
         <v>3.3418173687002152E-2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D5" si="1">C3*180/PI()</f>
+        <f t="shared" ref="D3:D5" si="1">DEGREES(C3)</f>
         <v>1.9147203113003646</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="2">A3*$A$10/(2*B3*TAN($A$11/2))</f>
+        <v>11.26997917626781</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>45</v>
       </c>
@@ -2379,8 +2414,15 @@
         <f t="shared" si="1"/>
         <v>1.8668225775521008</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>10.988004202784836</v>
+      </c>
+      <c r="F4">
+        <v>11.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -2394,6 +2436,35 @@
       <c r="D5">
         <f t="shared" si="1"/>
         <v>1.8710218101873164</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>11.012725019265446</v>
+      </c>
+      <c r="F5">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>640</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>RADIANS(87)</f>
+        <v>1.5184364492350666</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added max resolvable distance equation (see page 63 of notebook)
</commit_message>
<xml_diff>
--- a/results/marker_sizing/24-03-18_marker-sizing-test/24-03-18_marker-size-test-data.xlsx
+++ b/results/marker_sizing/24-03-18_marker-sizing-test/24-03-18_marker-size-test-data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\documents\uvm\5_masters\hive\github_directory\results\marker_sizing\24-03-18_marker-sizing-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52251818-BFC5-4F25-A082-CBEF155495D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF5BC76-F6DB-47E9-8564-DE11BE6C9206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13275" yWindow="20070" windowWidth="21600" windowHeight="11385" xr2:uid="{8CE0953D-CCFE-4D6F-99ED-C5F9A62F855B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{8CE0953D-CCFE-4D6F-99ED-C5F9A62F855B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>angle at max [deg]</t>
   </si>
@@ -63,6 +64,27 @@
   </si>
   <si>
     <t>actual pixel size (counted from image)</t>
+  </si>
+  <si>
+    <t>width of image</t>
+  </si>
+  <si>
+    <t>minimum resolvable pixel width</t>
+  </si>
+  <si>
+    <t>theta fov</t>
+  </si>
+  <si>
+    <t>marker size</t>
+  </si>
+  <si>
+    <t>expected max distance resolvable</t>
+  </si>
+  <si>
+    <t>actual max resolved</t>
+  </si>
+  <si>
+    <t>% error</t>
   </si>
 </sst>
 </file>
@@ -98,8 +120,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,6 +846,427 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>expected max distance resolvable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>919.66265479065805</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1164.9060294015003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1379.4939821859871</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1532.7710913177634</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-138C-48B2-8C92-8F9795ABC089}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>actual max resolved</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$2:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1381</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-138C-48B2-8C92-8F9795ABC089}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="613487888"/>
+        <c:axId val="613491488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="613487888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="613491488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="613491488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="800"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="613487888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -899,6 +1347,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1416,6 +1904,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2000,6 +3004,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB8B509B-84BA-638C-7BCC-5729C4D72E9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2327,8 +3372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E525651-0775-4550-ACDA-40153B2C3039}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,4 +3516,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FDFB9F-E760-4316-A543-C0C4B4ECF872}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>640</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*$A$1/(2*$A$2*TAN($A$3/2))</f>
+        <v>919.66265479065805</v>
+      </c>
+      <c r="H2">
+        <v>886</v>
+      </c>
+      <c r="I2" s="1">
+        <f>(G2-H2)/G2</f>
+        <v>3.6603263832998258E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>RADIANS(87)</f>
+        <v>1.5184364492350666</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G5" si="0">F3*$A$1/(2*$A$2*TAN($A$3/2))</f>
+        <v>1164.9060294015003</v>
+      </c>
+      <c r="H3">
+        <v>1137</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I5" si="1">(G3-H3)/G3</f>
+        <v>2.3955605600082364E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>1379.4939821859871</v>
+      </c>
+      <c r="H4">
+        <v>1381</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.0917175670650194E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>1532.7710913177634</v>
+      </c>
+      <c r="H5">
+        <v>1531</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1554832471695219E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
removed cloud averaging, fixed some bugs in main
</commit_message>
<xml_diff>
--- a/results/marker_sizing/24-03-18_marker-sizing-test/24-03-18_marker-size-test-data.xlsx
+++ b/results/marker_sizing/24-03-18_marker-sizing-test/24-03-18_marker-size-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\documents\uvm\5_masters\hive\github_directory\results\marker_sizing\24-03-18_marker-sizing-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF5BC76-F6DB-47E9-8564-DE11BE6C9206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E74D03-6BF0-4940-844E-1918AEC82E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{8CE0953D-CCFE-4D6F-99ED-C5F9A62F855B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{8CE0953D-CCFE-4D6F-99ED-C5F9A62F855B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3372,8 +3372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E525651-0775-4550-ACDA-40153B2C3039}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3522,7 +3522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FDFB9F-E760-4316-A543-C0C4B4ECF872}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>

</xml_diff>